<commit_message>
Reinserción de reporte quincenal
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceLGNEnergIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceLGNEnergIV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24D5F85-F5AE-4B33-B7F5-2BB0A2318A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FDCAAD-499A-49C7-B686-3C56C36A0C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,15 +71,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>LOTE IV</t>
   </si>
   <si>
     <t>MES:</t>
-  </si>
-  <si>
-    <t>NOVIEMBRE</t>
   </si>
   <si>
     <t>DÍA</t>
@@ -151,6 +148,18 @@
   </si>
   <si>
     <t>2ra Quincena</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.Mes}}</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.Anio}}</t>
+  </si>
+  <si>
+    <t>1RA QUINCENA {{dataResultResumen.Mes}}-{{dataResultResumen.Anio}}</t>
+  </si>
+  <si>
+    <t>2DA QUINCENA {{dataResultResumen.Mes}}-{{dataResultResumen.Anio}}</t>
   </si>
 </sst>
 </file>
@@ -161,7 +170,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +246,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -481,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -504,36 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -550,17 +537,8 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -573,18 +551,60 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,7 +889,7 @@
   <dimension ref="B2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,87 +905,87 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+    </row>
+    <row r="6" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="C6" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="29"/>
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="6" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" spans="2:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="J7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -996,280 +1016,293 @@
     </row>
     <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
+      <c r="B12" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
+      <c r="B13" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
     <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D19" s="43"/>
+      <c r="F19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="20" t="s">
-        <v>24</v>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="34" t="s">
+        <v>23</v>
       </c>
       <c r="K19" s="39"/>
       <c r="L19" s="40"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="15"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24" t="s">
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="26"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="24" t="s">
+      <c r="K21" s="15"/>
+      <c r="L21" s="14"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24" t="s">
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F22" s="24" t="s">
+      <c r="K22" s="15"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="24" t="s">
+      <c r="G23" s="17"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="27"/>
-      <c r="L22" s="26"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="28" t="s">
+      <c r="K23" s="15"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24" t="s">
+      <c r="G24" s="38"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="27"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F24" s="30" t="s">
+      <c r="K24" s="41"/>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F25" s="19"/>
+      <c r="G25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="30" t="s">
+      <c r="H25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="33"/>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="34"/>
-      <c r="G25" s="21" t="s">
+      <c r="L25" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="22" t="s">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F26" s="19"/>
+      <c r="G26" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="42" t="s">
+      <c r="H26" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="34"/>
-      <c r="G26" s="35" t="s">
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F27" s="19"/>
+      <c r="G27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="35" t="s">
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L26" s="35" t="s">
+      <c r="L27" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="34"/>
-      <c r="G27" s="35" t="s">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F28" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="L27" s="35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:L4"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="J6:L6"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>